<commit_message>
Strategy update, details in components.xlsx and daily_updates.txt
</commit_message>
<xml_diff>
--- a/docs/components.xlsx
+++ b/docs/components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NAM4SF\Documents\github\adaptive-cruise-control\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411DFB8F-5895-40F7-AE28-B63C7C4CA10D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E778E9-10FA-4C04-A844-301E986A5F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{93B556B3-0F1F-4620-A79F-3801F45D6D88}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="71">
   <si>
     <t>Item</t>
   </si>
@@ -240,9 +240,6 @@
     <t>https://www.mouser.bg/ProductDetail/Riverdi/RVT70HSMFWN00?qs=7D1LtPJG0i2G%2FPnN%252BYe%252ByQ%3D%3D&amp;_gl=1*1o1jhe3*_ga*NjY4NjA0NDcxLjE2OTM4OTYyODQ.*_ga_1KQLCYKRX3*MTY5NDA3MDUyOS4yLjAuMTY5NDA3MDUzNi41My4wLjA.*_ga_15W4STQT4T*MTY5NDA3MDUyOS4yLjAuMTY5NDA3MDUzNi4wLjAuMA..</t>
   </si>
   <si>
-    <t>Variant 1b (4 GB RAM) &lt;- Предлагам този</t>
-  </si>
-  <si>
     <t>Additional Components</t>
   </si>
   <si>
@@ -256,6 +253,18 @@
   </si>
   <si>
     <t>2 x Dynamode M-1100M</t>
+  </si>
+  <si>
+    <t>Variant 1b (4 GB RAM)</t>
+  </si>
+  <si>
+    <t>Variant 1c &lt;- Май този ще се наложи</t>
+  </si>
+  <si>
+    <t>RasPI CM4 Lite 2 GB</t>
+  </si>
+  <si>
+    <t>&lt;- Аз го купувам</t>
   </si>
 </sst>
 </file>
@@ -451,7 +460,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -506,18 +515,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -530,10 +548,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
@@ -924,7 +942,7 @@
   <dimension ref="A3:T54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="P37" sqref="P37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -934,47 +952,49 @@
     <col min="7" max="7" width="11" customWidth="1"/>
     <col min="8" max="8" width="15.44140625" style="2" customWidth="1"/>
     <col min="9" max="9" width="14.88671875" customWidth="1"/>
+    <col min="12" max="12" width="13.44140625" customWidth="1"/>
+    <col min="13" max="13" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26" t="s">
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26" t="s">
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26" t="s">
+      <c r="I3" s="29"/>
+      <c r="J3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="22" t="s">
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="T3" s="22"/>
+      <c r="T3" s="26"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
       <c r="E4" s="14" t="s">
         <v>1</v>
       </c>
@@ -990,34 +1010,34 @@
       <c r="I4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="22"/>
-      <c r="T4" s="22"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
     </row>
     <row r="5" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>1</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="25">
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="28">
         <v>5</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="28">
         <v>1800</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="28">
         <f xml:space="preserve"> E5*F5/1000</f>
         <v>9</v>
       </c>
@@ -1028,34 +1048,34 @@
         <f xml:space="preserve"> H5*1.95</f>
         <v>134.54999999999998</v>
       </c>
-      <c r="J5" s="28" t="s">
+      <c r="J5" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="23" t="s">
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="T5" s="23"/>
+      <c r="T5" s="25"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>2</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
       <c r="H6" s="6">
         <v>46</v>
       </c>
@@ -1063,38 +1083,38 @@
         <f t="shared" ref="I6:I16" si="0" xml:space="preserve"> H6*1.95</f>
         <v>89.7</v>
       </c>
-      <c r="J6" s="28" t="s">
+      <c r="J6" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="29"/>
-      <c r="S6" s="23" t="s">
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="31"/>
+      <c r="S6" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="T6" s="23"/>
+      <c r="T6" s="25"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="25">
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="28">
         <v>12</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="28">
         <v>0</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="28">
         <f t="shared" ref="G7" si="1" xml:space="preserve"> E7*F7/1000</f>
         <v>0</v>
       </c>
@@ -1105,32 +1125,32 @@
         <f t="shared" si="0"/>
         <v>62.750999999999998</v>
       </c>
-      <c r="J7" s="28" t="s">
+      <c r="J7" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="29"/>
-      <c r="S7" s="23" t="s">
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="31"/>
+      <c r="S7" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="T7" s="23"/>
+      <c r="T7" s="25"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>4</v>
       </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
       <c r="H8" s="6">
         <f>61.74 / 2</f>
         <v>30.87</v>
@@ -1138,38 +1158,38 @@
       <c r="I8" s="15">
         <v>61.74</v>
       </c>
-      <c r="J8" s="28" t="s">
+      <c r="J8" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="29"/>
-      <c r="S8" s="20" t="s">
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="31"/>
+      <c r="S8" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="T8" s="20"/>
+      <c r="T8" s="23"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>5</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="25">
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="28">
         <v>3.3</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="28">
         <v>300</v>
       </c>
-      <c r="G9" s="25">
+      <c r="G9" s="28">
         <f t="shared" ref="G9:G13" si="2" xml:space="preserve"> E9*F9/1000</f>
         <v>0.99</v>
       </c>
@@ -1180,32 +1200,32 @@
         <f t="shared" si="0"/>
         <v>27.358499999999999</v>
       </c>
-      <c r="J9" s="28" t="s">
+      <c r="J9" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="29"/>
-      <c r="S9" s="20" t="s">
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
+      <c r="P9" s="31"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="T9" s="20"/>
+      <c r="T9" s="23"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>6</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
       <c r="H10" s="6">
         <f>I10/1.95</f>
         <v>13.569230769230771</v>
@@ -1213,38 +1233,38 @@
       <c r="I10" s="15">
         <v>26.46</v>
       </c>
-      <c r="J10" s="28" t="s">
+      <c r="J10" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="29"/>
-      <c r="S10" s="20" t="s">
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="T10" s="20"/>
+      <c r="T10" s="23"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>7</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="25">
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="28">
         <v>5.0999999999999996</v>
       </c>
-      <c r="F11" s="25">
+      <c r="F11" s="28">
         <v>850</v>
       </c>
-      <c r="G11" s="25">
+      <c r="G11" s="28">
         <f t="shared" si="2"/>
         <v>4.335</v>
       </c>
@@ -1255,32 +1275,32 @@
       <c r="I11" s="15">
         <v>146.58000000000001</v>
       </c>
-      <c r="J11" s="28" t="s">
+      <c r="J11" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="29"/>
-      <c r="P11" s="29"/>
-      <c r="Q11" s="29"/>
-      <c r="R11" s="29"/>
-      <c r="S11" s="20" t="s">
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="31"/>
+      <c r="R11" s="31"/>
+      <c r="S11" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="T11" s="20"/>
+      <c r="T11" s="23"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>8</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
       <c r="H12" s="6">
         <f>I12/1.95</f>
         <v>49.261538461538464</v>
@@ -1288,38 +1308,38 @@
       <c r="I12" s="15">
         <v>96.06</v>
       </c>
-      <c r="J12" s="30" t="s">
+      <c r="J12" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="30"/>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="30"/>
-      <c r="R12" s="30"/>
-      <c r="S12" s="23" t="s">
+      <c r="K12" s="33"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="33"/>
+      <c r="O12" s="33"/>
+      <c r="P12" s="33"/>
+      <c r="Q12" s="33"/>
+      <c r="R12" s="33"/>
+      <c r="S12" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="T12" s="23"/>
+      <c r="T12" s="25"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>9</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="25">
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="28">
         <v>0</v>
       </c>
-      <c r="F13" s="25">
+      <c r="F13" s="28">
         <v>0</v>
       </c>
-      <c r="G13" s="25">
+      <c r="G13" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1330,32 +1350,32 @@
       <c r="I13" s="15">
         <v>5.9</v>
       </c>
-      <c r="J13" s="28" t="s">
+      <c r="J13" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="29"/>
-      <c r="R13" s="29"/>
-      <c r="S13" s="20" t="s">
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="31"/>
+      <c r="R13" s="31"/>
+      <c r="S13" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="T13" s="20"/>
+      <c r="T13" s="23"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>10</v>
       </c>
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
       <c r="H14" s="6">
         <f>I14/1.95</f>
         <v>1.4871794871794872</v>
@@ -1363,38 +1383,38 @@
       <c r="I14" s="15">
         <v>2.9</v>
       </c>
-      <c r="J14" s="28" t="s">
+      <c r="J14" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29"/>
-      <c r="O14" s="29"/>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="29"/>
-      <c r="R14" s="29"/>
-      <c r="S14" s="20" t="s">
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="31"/>
+      <c r="P14" s="31"/>
+      <c r="Q14" s="31"/>
+      <c r="R14" s="31"/>
+      <c r="S14" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="T14" s="20"/>
+      <c r="T14" s="23"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>11</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="25" t="s">
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="25" t="s">
+      <c r="F15" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="25" t="s">
+      <c r="G15" s="28" t="s">
         <v>24</v>
       </c>
       <c r="H15" s="6">
@@ -1404,32 +1424,32 @@
         <f t="shared" si="0"/>
         <v>7.1760000000000002</v>
       </c>
-      <c r="J15" s="28" t="s">
+      <c r="J15" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="29"/>
-      <c r="O15" s="29"/>
-      <c r="P15" s="29"/>
-      <c r="Q15" s="29"/>
-      <c r="R15" s="29"/>
-      <c r="S15" s="20" t="s">
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="31"/>
+      <c r="Q15" s="31"/>
+      <c r="R15" s="31"/>
+      <c r="S15" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="T15" s="20"/>
+      <c r="T15" s="23"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>12</v>
       </c>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
       <c r="H16" s="6">
         <v>7.73</v>
       </c>
@@ -1437,29 +1457,29 @@
         <f t="shared" si="0"/>
         <v>15.073500000000001</v>
       </c>
-      <c r="J16" s="28" t="s">
+      <c r="J16" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="29"/>
-      <c r="O16" s="29"/>
-      <c r="P16" s="29"/>
-      <c r="Q16" s="29"/>
-      <c r="R16" s="29"/>
-      <c r="S16" s="20" t="s">
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="31"/>
+      <c r="P16" s="31"/>
+      <c r="Q16" s="31"/>
+      <c r="R16" s="31"/>
+      <c r="S16" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="T16" s="20"/>
+      <c r="T16" s="23"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
       <c r="E17" s="13" t="s">
         <v>24</v>
       </c>
@@ -1471,30 +1491,30 @@
         <f>SUM(G5:G14)</f>
         <v>14.324999999999999</v>
       </c>
-      <c r="H17" s="33" t="s">
+      <c r="H17" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="I17" s="33"/>
-      <c r="J17" s="29" t="s">
+      <c r="I17" s="36"/>
+      <c r="J17" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="29"/>
-      <c r="O17" s="29"/>
-      <c r="P17" s="29"/>
-      <c r="Q17" s="29"/>
-      <c r="R17" s="29"/>
-      <c r="S17" s="21" t="s">
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="31"/>
+      <c r="P17" s="31"/>
+      <c r="Q17" s="31"/>
+      <c r="R17" s="31"/>
+      <c r="S17" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="T17" s="21"/>
+      <c r="T17" s="24"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -1511,43 +1531,43 @@
       <c r="R18" s="11"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
       <c r="E19" s="4"/>
-      <c r="F19" s="24" t="s">
+      <c r="F19" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="24"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
       <c r="J19" s="11"/>
-      <c r="K19" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="26"/>
-      <c r="P19" s="26"/>
-      <c r="Q19" s="26"/>
-      <c r="R19" s="26"/>
-      <c r="S19" s="26"/>
-      <c r="T19" s="26"/>
+      <c r="K19" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="29"/>
+      <c r="R19" s="29"/>
+      <c r="S19" s="29"/>
+      <c r="T19" s="29"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
       <c r="E20" s="4"/>
-      <c r="F20" s="24" t="s">
+      <c r="F20" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="G20" s="24"/>
+      <c r="G20" s="27"/>
       <c r="H20" s="8" t="s">
         <v>33</v>
       </c>
@@ -1555,34 +1575,34 @@
         <v>34</v>
       </c>
       <c r="J20" s="11"/>
-      <c r="K20" s="26" t="s">
+      <c r="K20" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="L20" s="26"/>
-      <c r="M20" s="26" t="s">
+      <c r="L20" s="29"/>
+      <c r="M20" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="N20" s="26"/>
-      <c r="O20" s="26" t="s">
+      <c r="N20" s="29"/>
+      <c r="O20" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P20" s="26"/>
-      <c r="Q20" s="26"/>
-      <c r="R20" s="26"/>
-      <c r="S20" s="26"/>
-      <c r="T20" s="26"/>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="29"/>
+      <c r="R20" s="29"/>
+      <c r="S20" s="29"/>
+      <c r="T20" s="29"/>
     </row>
     <row r="21" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="25" t="s">
+      <c r="F21" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="G21" s="25"/>
+      <c r="G21" s="28"/>
       <c r="H21" s="6">
         <v>134.55000000000001</v>
       </c>
@@ -1590,32 +1610,32 @@
         <v>1</v>
       </c>
       <c r="J21" s="11"/>
-      <c r="K21" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="L21" s="29"/>
-      <c r="M21" s="29">
+      <c r="K21" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="L21" s="31"/>
+      <c r="M21" s="31">
         <v>22.91</v>
       </c>
-      <c r="N21" s="29"/>
-      <c r="O21" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="P21" s="29"/>
-      <c r="Q21" s="29"/>
-      <c r="R21" s="29"/>
-      <c r="S21" s="29"/>
-      <c r="T21" s="29"/>
+      <c r="N21" s="31"/>
+      <c r="O21" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="P21" s="31"/>
+      <c r="Q21" s="31"/>
+      <c r="R21" s="31"/>
+      <c r="S21" s="31"/>
+      <c r="T21" s="31"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
       <c r="E22" s="4"/>
-      <c r="F22" s="25" t="s">
+      <c r="F22" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="G22" s="25"/>
+      <c r="G22" s="28"/>
       <c r="H22" s="6">
         <v>61.74</v>
       </c>
@@ -1633,14 +1653,14 @@
       <c r="R22" s="11"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B23" s="31"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="G23" s="25"/>
+      <c r="F23" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" s="28"/>
       <c r="H23" s="6">
         <f>14.03 * 2</f>
         <v>28.06</v>
@@ -1659,16 +1679,16 @@
       <c r="R23" s="11"/>
     </row>
     <row r="24" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
       <c r="E24" s="4"/>
-      <c r="F24" s="25" t="s">
+      <c r="F24" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="G24" s="25"/>
+      <c r="G24" s="28"/>
       <c r="H24" s="6">
         <v>96.06</v>
       </c>
@@ -1686,14 +1706,14 @@
       <c r="R24" s="11"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
       <c r="E25" s="4"/>
-      <c r="F25" s="25" t="s">
+      <c r="F25" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="G25" s="25"/>
+      <c r="G25" s="28"/>
       <c r="H25" s="6">
         <v>5.9</v>
       </c>
@@ -1711,14 +1731,14 @@
       <c r="R25" s="11"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B26" s="31"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
       <c r="E26" s="4"/>
-      <c r="F26" s="25" t="s">
+      <c r="F26" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="G26" s="25"/>
+      <c r="G26" s="28"/>
       <c r="H26" s="6">
         <v>7.17</v>
       </c>
@@ -1736,14 +1756,14 @@
       <c r="R26" s="11"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
       <c r="E27" s="4"/>
-      <c r="F27" s="24" t="s">
+      <c r="F27" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="G27" s="24"/>
+      <c r="G27" s="27"/>
       <c r="H27" s="6">
         <f>SUM(H21:H26)</f>
         <v>333.48</v>
@@ -1762,9 +1782,9 @@
       <c r="R27" s="11"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
@@ -1781,35 +1801,37 @@
       <c r="R28" s="11"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
       <c r="E29" s="4"/>
-      <c r="F29" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="24"/>
+      <c r="F29" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
       <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
-      <c r="L29" s="11"/>
-      <c r="M29" s="11"/>
-      <c r="N29" s="11"/>
+      <c r="K29" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="L29" s="27"/>
+      <c r="M29" s="27"/>
+      <c r="N29" s="27"/>
       <c r="O29" s="11"/>
       <c r="P29" s="11"/>
       <c r="Q29" s="11"/>
       <c r="R29" s="11"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
       <c r="E30" s="4"/>
-      <c r="F30" s="24" t="s">
+      <c r="F30" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="G30" s="24"/>
+      <c r="G30" s="27"/>
       <c r="H30" s="8" t="s">
         <v>33</v>
       </c>
@@ -1817,24 +1839,30 @@
         <v>34</v>
       </c>
       <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="11"/>
-      <c r="N30" s="11"/>
+      <c r="K30" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="L30" s="27"/>
+      <c r="M30" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="N30" s="21" t="s">
+        <v>34</v>
+      </c>
       <c r="O30" s="11"/>
       <c r="P30" s="11"/>
       <c r="Q30" s="11"/>
       <c r="R30" s="11"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
       <c r="E31" s="4"/>
-      <c r="F31" s="25" t="s">
+      <c r="F31" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="G31" s="25"/>
+      <c r="G31" s="28"/>
       <c r="H31" s="6">
         <v>89.7</v>
       </c>
@@ -1842,24 +1870,32 @@
         <v>1</v>
       </c>
       <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="11"/>
-      <c r="M31" s="11"/>
-      <c r="N31" s="11"/>
-      <c r="O31" s="11"/>
+      <c r="K31" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="L31" s="28"/>
+      <c r="M31" s="6">
+        <v>0</v>
+      </c>
+      <c r="N31" s="20">
+        <v>1</v>
+      </c>
+      <c r="O31" s="11" t="s">
+        <v>70</v>
+      </c>
       <c r="P31" s="11"/>
       <c r="Q31" s="11"/>
       <c r="R31" s="11"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
       <c r="E32" s="4"/>
-      <c r="F32" s="25" t="s">
+      <c r="F32" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="G32" s="25"/>
+      <c r="G32" s="28"/>
       <c r="H32" s="6">
         <v>61.74</v>
       </c>
@@ -1867,24 +1903,30 @@
         <v>4</v>
       </c>
       <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
-      <c r="L32" s="11"/>
-      <c r="M32" s="11"/>
-      <c r="N32" s="11"/>
+      <c r="K32" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="L32" s="28"/>
+      <c r="M32" s="6">
+        <v>61.74</v>
+      </c>
+      <c r="N32" s="20">
+        <v>4</v>
+      </c>
       <c r="O32" s="11"/>
       <c r="P32" s="11"/>
       <c r="Q32" s="11"/>
       <c r="R32" s="11"/>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
       <c r="E33" s="4"/>
-      <c r="F33" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="G33" s="25"/>
+      <c r="F33" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G33" s="28"/>
       <c r="H33" s="6">
         <f xml:space="preserve"> 14.03 * 2</f>
         <v>28.06</v>
@@ -1893,24 +1935,31 @@
         <v>5</v>
       </c>
       <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="11"/>
-      <c r="M33" s="11"/>
-      <c r="N33" s="11"/>
+      <c r="K33" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="L33" s="28"/>
+      <c r="M33" s="6">
+        <f xml:space="preserve"> 14.03 * 2</f>
+        <v>28.06</v>
+      </c>
+      <c r="N33" s="20">
+        <v>5</v>
+      </c>
       <c r="O33" s="11"/>
       <c r="P33" s="11"/>
       <c r="Q33" s="11"/>
       <c r="R33" s="11"/>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
       <c r="E34" s="4"/>
-      <c r="F34" s="25" t="s">
+      <c r="F34" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="25"/>
+      <c r="G34" s="28"/>
       <c r="H34" s="6">
         <v>98.65</v>
       </c>
@@ -1918,26 +1967,32 @@
         <v>7</v>
       </c>
       <c r="J34" s="11"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="11"/>
-      <c r="M34" s="11"/>
-      <c r="N34" s="11"/>
+      <c r="K34" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="L34" s="28"/>
+      <c r="M34" s="6">
+        <v>96.06</v>
+      </c>
+      <c r="N34" s="20">
+        <v>7</v>
+      </c>
       <c r="O34" s="11"/>
       <c r="P34" s="11"/>
       <c r="Q34" s="11"/>
       <c r="R34" s="11"/>
     </row>
     <row r="35" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="31" t="s">
+      <c r="B35" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
       <c r="E35" s="4"/>
-      <c r="F35" s="25" t="s">
+      <c r="F35" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="G35" s="25"/>
+      <c r="G35" s="28"/>
       <c r="H35" s="6">
         <v>5.9</v>
       </c>
@@ -1945,24 +2000,30 @@
         <v>9</v>
       </c>
       <c r="J35" s="11"/>
-      <c r="K35" s="11"/>
-      <c r="L35" s="11"/>
-      <c r="M35" s="11"/>
-      <c r="N35" s="11"/>
+      <c r="K35" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="L35" s="28"/>
+      <c r="M35" s="6">
+        <v>5.9</v>
+      </c>
+      <c r="N35" s="20">
+        <v>9</v>
+      </c>
       <c r="O35" s="11"/>
       <c r="P35" s="11"/>
       <c r="Q35" s="11"/>
       <c r="R35" s="11"/>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
       <c r="E36" s="4"/>
-      <c r="F36" s="25" t="s">
+      <c r="F36" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="G36" s="25"/>
+      <c r="G36" s="28"/>
       <c r="H36" s="6">
         <v>7.17</v>
       </c>
@@ -1970,24 +2031,30 @@
         <v>11</v>
       </c>
       <c r="J36" s="11"/>
-      <c r="K36" s="11"/>
-      <c r="L36" s="11"/>
-      <c r="M36" s="11"/>
-      <c r="N36" s="11"/>
+      <c r="K36" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="L36" s="28"/>
+      <c r="M36" s="6">
+        <v>7.17</v>
+      </c>
+      <c r="N36" s="20">
+        <v>11</v>
+      </c>
       <c r="O36" s="11"/>
       <c r="P36" s="11"/>
       <c r="Q36" s="11"/>
       <c r="R36" s="11"/>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B37" s="31"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
       <c r="E37" s="4"/>
-      <c r="F37" s="24" t="s">
+      <c r="F37" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="G37" s="24"/>
+      <c r="G37" s="27"/>
       <c r="H37" s="6">
         <f>SUM(H31:H36, M21)</f>
         <v>314.13</v>
@@ -1996,19 +2063,26 @@
         <v>39</v>
       </c>
       <c r="J37" s="11"/>
-      <c r="K37" s="11"/>
-      <c r="L37" s="11"/>
-      <c r="M37" s="11"/>
-      <c r="N37" s="11"/>
+      <c r="K37" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="L37" s="27"/>
+      <c r="M37" s="6">
+        <f>SUM(M31:M36, M21)</f>
+        <v>221.84</v>
+      </c>
+      <c r="N37" s="20" t="s">
+        <v>39</v>
+      </c>
       <c r="O37" s="11"/>
       <c r="P37" s="11"/>
       <c r="Q37" s="11"/>
       <c r="R37" s="11"/>
     </row>
     <row r="38" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B38" s="31"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="31"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="34"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
@@ -2025,9 +2099,9 @@
       <c r="R38" s="11"/>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
@@ -2317,7 +2391,16 @@
       <c r="D54" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="90">
+  <mergeCells count="99">
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="K29:N29"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="K33:L33"/>
     <mergeCell ref="K21:L21"/>
     <mergeCell ref="O21:T21"/>
     <mergeCell ref="M21:N21"/>
@@ -2447,44 +2530,44 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26" t="s">
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26" t="s">
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26" t="s">
+      <c r="I3" s="29"/>
+      <c r="J3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="22" t="s">
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="T3" s="22"/>
+      <c r="T3" s="26"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
       <c r="E4" s="14" t="s">
         <v>1</v>
       </c>
@@ -2500,34 +2583,34 @@
       <c r="I4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="22"/>
-      <c r="T4" s="22"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
     </row>
     <row r="5" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="36">
+      <c r="A5" s="39">
         <v>1</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="25">
+      <c r="C5" s="42"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="28">
         <v>5</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="28">
         <v>3000</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="28">
         <f xml:space="preserve"> E5*F5/1000</f>
         <v>15</v>
       </c>
@@ -2538,30 +2621,30 @@
         <f xml:space="preserve"> H5*1.95</f>
         <v>134.47199999999998</v>
       </c>
-      <c r="J5" s="28" t="s">
+      <c r="J5" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="23" t="s">
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="T5" s="23"/>
+      <c r="T5" s="25"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" s="37"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
+      <c r="A6" s="40"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
       <c r="H6" s="6">
         <v>56</v>
       </c>
@@ -2569,31 +2652,31 @@
         <f t="shared" ref="I6:I14" si="0" xml:space="preserve"> H6*1.95</f>
         <v>109.2</v>
       </c>
-      <c r="J6" s="28" t="s">
+      <c r="J6" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="29"/>
-      <c r="S6" s="23" t="s">
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="31"/>
+      <c r="S6" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="T6" s="23"/>
+      <c r="T6" s="25"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>2</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
       <c r="E7" s="12">
         <v>5</v>
       </c>
@@ -2611,31 +2694,31 @@
         <f t="shared" si="0"/>
         <v>45.103499999999997</v>
       </c>
-      <c r="J7" s="28" t="s">
+      <c r="J7" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="29"/>
-      <c r="S7" s="20" t="s">
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="31"/>
+      <c r="S7" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="T7" s="20"/>
+      <c r="T7" s="23"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>3</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
       <c r="E8" s="12">
         <v>5</v>
       </c>
@@ -2653,38 +2736,38 @@
         <f t="shared" si="0"/>
         <v>29.503500000000003</v>
       </c>
-      <c r="J8" s="28" t="s">
+      <c r="J8" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="29"/>
-      <c r="S8" s="20" t="s">
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="31"/>
+      <c r="S8" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="T8" s="20"/>
+      <c r="T8" s="23"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>4</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="25">
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="28">
         <v>5.0999999999999996</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="28">
         <v>850</v>
       </c>
-      <c r="G9" s="25">
+      <c r="G9" s="28">
         <f t="shared" ref="G9:G11" si="2" xml:space="preserve"> E9*F9/1000</f>
         <v>4.335</v>
       </c>
@@ -2695,32 +2778,32 @@
       <c r="I9" s="15">
         <v>146.58000000000001</v>
       </c>
-      <c r="J9" s="28" t="s">
+      <c r="J9" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="29"/>
-      <c r="S9" s="20" t="s">
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
+      <c r="P9" s="31"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="T9" s="20"/>
+      <c r="T9" s="23"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>5</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
       <c r="H10" s="6">
         <f>I10/1.95</f>
         <v>50.589743589743591</v>
@@ -2728,38 +2811,38 @@
       <c r="I10" s="15">
         <v>98.65</v>
       </c>
-      <c r="J10" s="30" t="s">
+      <c r="J10" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="29"/>
-      <c r="S10" s="20" t="s">
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="T10" s="20"/>
+      <c r="T10" s="23"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>6</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="25">
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="28">
         <v>0</v>
       </c>
-      <c r="F11" s="25">
+      <c r="F11" s="28">
         <v>0</v>
       </c>
-      <c r="G11" s="25">
+      <c r="G11" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2770,32 +2853,32 @@
       <c r="I11" s="15">
         <v>5.9</v>
       </c>
-      <c r="J11" s="28" t="s">
+      <c r="J11" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="29"/>
-      <c r="P11" s="29"/>
-      <c r="Q11" s="29"/>
-      <c r="R11" s="29"/>
-      <c r="S11" s="20" t="s">
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="31"/>
+      <c r="R11" s="31"/>
+      <c r="S11" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="T11" s="20"/>
+      <c r="T11" s="23"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>7</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
       <c r="H12" s="6">
         <f>I12/1.95</f>
         <v>1.4871794871794872</v>
@@ -2803,38 +2886,38 @@
       <c r="I12" s="15">
         <v>2.9</v>
       </c>
-      <c r="J12" s="28" t="s">
+      <c r="J12" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="29"/>
-      <c r="S12" s="20" t="s">
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="31"/>
+      <c r="Q12" s="31"/>
+      <c r="R12" s="31"/>
+      <c r="S12" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="T12" s="20"/>
+      <c r="T12" s="23"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>8</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="25" t="s">
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="25" t="s">
+      <c r="F13" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="25" t="s">
+      <c r="G13" s="28" t="s">
         <v>24</v>
       </c>
       <c r="H13" s="6">
@@ -2844,32 +2927,32 @@
         <f t="shared" si="0"/>
         <v>36.270000000000003</v>
       </c>
-      <c r="J13" s="28" t="s">
+      <c r="J13" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="29"/>
-      <c r="R13" s="29"/>
-      <c r="S13" s="23" t="s">
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="31"/>
+      <c r="R13" s="31"/>
+      <c r="S13" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="T13" s="23"/>
+      <c r="T13" s="25"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>9</v>
       </c>
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
       <c r="H14" s="6">
         <v>7.73</v>
       </c>
@@ -2877,29 +2960,29 @@
         <f t="shared" si="0"/>
         <v>15.073500000000001</v>
       </c>
-      <c r="J14" s="28" t="s">
+      <c r="J14" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29"/>
-      <c r="O14" s="29"/>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="29"/>
-      <c r="R14" s="29"/>
-      <c r="S14" s="20" t="s">
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="31"/>
+      <c r="P14" s="31"/>
+      <c r="Q14" s="31"/>
+      <c r="R14" s="31"/>
+      <c r="S14" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="T14" s="20"/>
+      <c r="T14" s="23"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="17"/>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
       <c r="E15" s="13" t="s">
         <v>24</v>
       </c>
@@ -2911,32 +2994,32 @@
         <f>SUM(G5:G12)</f>
         <v>22.335000000000001</v>
       </c>
-      <c r="H15" s="33" t="s">
+      <c r="H15" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="33"/>
-      <c r="J15" s="29" t="s">
+      <c r="I15" s="36"/>
+      <c r="J15" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="29"/>
-      <c r="O15" s="29"/>
-      <c r="P15" s="29"/>
-      <c r="Q15" s="29"/>
-      <c r="R15" s="29"/>
-      <c r="S15" s="21" t="s">
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="31"/>
+      <c r="Q15" s="31"/>
+      <c r="R15" s="31"/>
+      <c r="S15" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="T15" s="21"/>
+      <c r="T15" s="24"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="18" t="s">
@@ -2962,7 +3045,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C20" s="10">
         <f>29.5*2</f>

</xml_diff>

<commit_message>
Minor update, written in docs
</commit_message>
<xml_diff>
--- a/docs/components.xlsx
+++ b/docs/components.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NAM4SF\Documents\github\adaptive-cruise-control\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E778E9-10FA-4C04-A844-301E986A5F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897EF3CE-1C17-4186-8E46-216E5CC816C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{93B556B3-0F1F-4620-A79F-3801F45D6D88}"/>
   </bookViews>
   <sheets>
-    <sheet name="CM4_Vairant" sheetId="1" r:id="rId1"/>
-    <sheet name="RPI4_Variant" sheetId="2" r:id="rId2"/>
+    <sheet name="LinkList" sheetId="3" r:id="rId1"/>
+    <sheet name="CM4_Vairant" sheetId="1" r:id="rId2"/>
+    <sheet name="RPI4_Variant" sheetId="2" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="76">
   <si>
     <t>Item</t>
   </si>
@@ -234,9 +235,6 @@
     <t>https://www.tme.eu/bg/details/psd-30a-5/preobrazuvateli-dc-dc/mean-well/</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>https://www.mouser.bg/ProductDetail/Riverdi/RVT70HSMFWN00?qs=7D1LtPJG0i2G%2FPnN%252BYe%252ByQ%3D%3D&amp;_gl=1*1o1jhe3*_ga*NjY4NjA0NDcxLjE2OTM4OTYyODQ.*_ga_1KQLCYKRX3*MTY5NDA3MDUyOS4yLjAuMTY5NDA3MDUzNi41My4wLjA.*_ga_15W4STQT4T*MTY5NDA3MDUyOS4yLjAuMTY5NDA3MDUzNi4wLjAuMA..</t>
   </si>
   <si>
@@ -258,13 +256,31 @@
     <t>Variant 1b (4 GB RAM)</t>
   </si>
   <si>
-    <t>Variant 1c &lt;- Май този ще се наложи</t>
-  </si>
-  <si>
-    <t>RasPI CM4 Lite 2 GB</t>
-  </si>
-  <si>
-    <t>&lt;- Аз го купувам</t>
+    <t>https://buyzero.de/en/products/compute-module-4-cm4?variant=32090358251622</t>
+  </si>
+  <si>
+    <t>https://www.welectron.com/Raspberry-Pi-CM4002032-Compute-Module-32-GB-2-GB-RAM_1</t>
+  </si>
+  <si>
+    <t>Raspberry Pi Compute Module 4 (2 GB)</t>
+  </si>
+  <si>
+    <t>https://www.welectron.com/Raspberry-Pi-Compute-Module-CM4-IO-Board_1</t>
+  </si>
+  <si>
+    <t>https://de.riverdi.com/product/high-brightness-ips-display-rvt70hsmfwn00-7-zoll-mipi-dsi-frame</t>
+  </si>
+  <si>
+    <t>Availability (13.09.2023)</t>
+  </si>
+  <si>
+    <t>Display (SM-RVT70HSMFWN00)</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Order List</t>
   </si>
 </sst>
 </file>
@@ -460,7 +476,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -594,6 +610,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -938,11 +966,415 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD6834A-62F7-4E19-8029-A60D704C753F}">
+  <dimension ref="B2:S12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="17" max="17" width="19.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B2" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B3" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="S3" s="26"/>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+    </row>
+    <row r="5" spans="2:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="9">
+        <v>1</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="49">
+        <v>1</v>
+      </c>
+      <c r="G5" s="6">
+        <v>47.19</v>
+      </c>
+      <c r="H5" s="20">
+        <f xml:space="preserve"> G5*1.95</f>
+        <v>92.020499999999998</v>
+      </c>
+      <c r="I5" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="S5" s="23"/>
+    </row>
+    <row r="6" spans="2:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="9">
+        <v>2</v>
+      </c>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="6">
+        <v>62.9</v>
+      </c>
+      <c r="H6" s="20">
+        <f t="shared" ref="H6:H12" si="0" xml:space="preserve"> G6*1.95</f>
+        <v>122.655</v>
+      </c>
+      <c r="I6" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="S6" s="23"/>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B7" s="9">
+        <v>3</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="49">
+        <v>1</v>
+      </c>
+      <c r="G7" s="6">
+        <v>39.9</v>
+      </c>
+      <c r="H7" s="20">
+        <f t="shared" si="0"/>
+        <v>77.804999999999993</v>
+      </c>
+      <c r="I7" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="S7" s="23"/>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B8" s="9">
+        <v>4</v>
+      </c>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="6">
+        <f>61.74 / 2</f>
+        <v>30.87</v>
+      </c>
+      <c r="H8" s="20">
+        <v>61.74</v>
+      </c>
+      <c r="I8" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="S8" s="23"/>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B9" s="9">
+        <v>5</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="49">
+        <v>2</v>
+      </c>
+      <c r="G9" s="20">
+        <v>14.03</v>
+      </c>
+      <c r="H9" s="20">
+        <f t="shared" si="0"/>
+        <v>27.358499999999999</v>
+      </c>
+      <c r="I9" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
+      <c r="P9" s="31"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="S9" s="23"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B10" s="9">
+        <v>6</v>
+      </c>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="6">
+        <f>H10/1.95</f>
+        <v>13.569230769230771</v>
+      </c>
+      <c r="H10" s="20">
+        <v>26.46</v>
+      </c>
+      <c r="I10" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="S10" s="23"/>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B11" s="9">
+        <v>7</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="49">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6">
+        <f>H11/1.95</f>
+        <v>50.97948717948718</v>
+      </c>
+      <c r="H11" s="20">
+        <v>99.41</v>
+      </c>
+      <c r="I11" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="31"/>
+      <c r="R11" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="S11" s="23"/>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B12" s="9">
+        <v>8</v>
+      </c>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="6">
+        <f>H12/1.95</f>
+        <v>49.261538461538464</v>
+      </c>
+      <c r="H12" s="20">
+        <v>96.06</v>
+      </c>
+      <c r="I12" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="J12" s="33"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="33"/>
+      <c r="O12" s="33"/>
+      <c r="P12" s="33"/>
+      <c r="Q12" s="33"/>
+      <c r="R12" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="S12" s="23"/>
+    </row>
+  </sheetData>
+  <mergeCells count="31">
+    <mergeCell ref="B2:S2"/>
+    <mergeCell ref="C11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="I11:Q11"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="I12:Q12"/>
+    <mergeCell ref="R12:S12"/>
+    <mergeCell ref="C9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="I9:Q9"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="I10:Q10"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="C7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="I7:Q7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="I8:Q8"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="I5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="I6:Q6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="C5:E6"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:E4"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:Q4"/>
+    <mergeCell ref="R3:S4"/>
+    <mergeCell ref="F3:F4"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="I7" r:id="rId1" xr:uid="{4835562A-740E-44BF-972E-7EE1336F2F12}"/>
+    <hyperlink ref="I8" r:id="rId2" xr:uid="{1253BC12-3340-4C45-85EE-9F5745984BF6}"/>
+    <hyperlink ref="I9" r:id="rId3" xr:uid="{FE049DAA-A2C1-41BC-9339-1CAFB1FD8733}"/>
+    <hyperlink ref="I10" r:id="rId4" xr:uid="{5B9D5137-8E5C-4E79-BECE-1DC22045A466}"/>
+    <hyperlink ref="I11" r:id="rId5" xr:uid="{D49B211A-7F18-4283-AD45-589E80AB5DE0}"/>
+    <hyperlink ref="I12" r:id="rId6" xr:uid="{3210318C-9FF3-4760-96E3-1073438B4AF1}"/>
+    <hyperlink ref="I5" r:id="rId7" xr:uid="{8B756AC3-1B1C-4EF2-988A-5AC7F0F652B1}"/>
+    <hyperlink ref="I6" r:id="rId8" xr:uid="{4B92FE02-B3D1-4BFA-97F1-6A570E7F4701}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B714DB9D-3D94-4649-9B27-6954336A2F86}">
   <dimension ref="A3:T54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P37" sqref="P37"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1309,7 +1741,7 @@
         <v>96.06</v>
       </c>
       <c r="J12" s="33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K12" s="33"/>
       <c r="L12" s="33"/>
@@ -1545,7 +1977,7 @@
       <c r="I19" s="27"/>
       <c r="J19" s="11"/>
       <c r="K19" s="29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L19" s="29"/>
       <c r="M19" s="29"/>
@@ -1611,7 +2043,7 @@
       </c>
       <c r="J21" s="11"/>
       <c r="K21" s="31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L21" s="31"/>
       <c r="M21" s="31">
@@ -1619,7 +2051,7 @@
       </c>
       <c r="N21" s="31"/>
       <c r="O21" s="32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P21" s="31"/>
       <c r="Q21" s="31"/>
@@ -1658,7 +2090,7 @@
       <c r="D23" s="34"/>
       <c r="E23" s="4"/>
       <c r="F23" s="28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G23" s="28"/>
       <c r="H23" s="6">
@@ -1771,15 +2203,6 @@
       <c r="I27" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
-      <c r="N27" s="11"/>
-      <c r="O27" s="11"/>
-      <c r="P27" s="11"/>
-      <c r="Q27" s="11"/>
-      <c r="R27" s="11"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B28" s="34"/>
@@ -1790,15 +2213,6 @@
       <c r="G28" s="4"/>
       <c r="H28" s="3"/>
       <c r="I28" s="1"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
-      <c r="M28" s="11"/>
-      <c r="N28" s="11"/>
-      <c r="O28" s="11"/>
-      <c r="P28" s="11"/>
-      <c r="Q28" s="11"/>
-      <c r="R28" s="11"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B29" s="34"/>
@@ -1806,22 +2220,11 @@
       <c r="D29" s="34"/>
       <c r="E29" s="4"/>
       <c r="F29" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G29" s="27"/>
       <c r="H29" s="27"/>
       <c r="I29" s="27"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="L29" s="27"/>
-      <c r="M29" s="27"/>
-      <c r="N29" s="27"/>
-      <c r="O29" s="11"/>
-      <c r="P29" s="11"/>
-      <c r="Q29" s="11"/>
-      <c r="R29" s="11"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B30" s="34"/>
@@ -1838,21 +2241,6 @@
       <c r="I30" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J30" s="11"/>
-      <c r="K30" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="L30" s="27"/>
-      <c r="M30" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="N30" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="O30" s="11"/>
-      <c r="P30" s="11"/>
-      <c r="Q30" s="11"/>
-      <c r="R30" s="11"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B31" s="34"/>
@@ -1869,23 +2257,6 @@
       <c r="I31" s="7">
         <v>1</v>
       </c>
-      <c r="J31" s="11"/>
-      <c r="K31" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="L31" s="28"/>
-      <c r="M31" s="6">
-        <v>0</v>
-      </c>
-      <c r="N31" s="20">
-        <v>1</v>
-      </c>
-      <c r="O31" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="P31" s="11"/>
-      <c r="Q31" s="11"/>
-      <c r="R31" s="11"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B32" s="34"/>
@@ -1902,21 +2273,6 @@
       <c r="I32" s="7">
         <v>4</v>
       </c>
-      <c r="J32" s="11"/>
-      <c r="K32" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="L32" s="28"/>
-      <c r="M32" s="6">
-        <v>61.74</v>
-      </c>
-      <c r="N32" s="20">
-        <v>4</v>
-      </c>
-      <c r="O32" s="11"/>
-      <c r="P32" s="11"/>
-      <c r="Q32" s="11"/>
-      <c r="R32" s="11"/>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B33" s="34"/>
@@ -1924,7 +2280,7 @@
       <c r="D33" s="34"/>
       <c r="E33" s="4"/>
       <c r="F33" s="28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G33" s="28"/>
       <c r="H33" s="6">
@@ -1934,22 +2290,6 @@
       <c r="I33" s="7">
         <v>5</v>
       </c>
-      <c r="J33" s="11"/>
-      <c r="K33" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="L33" s="28"/>
-      <c r="M33" s="6">
-        <f xml:space="preserve"> 14.03 * 2</f>
-        <v>28.06</v>
-      </c>
-      <c r="N33" s="20">
-        <v>5</v>
-      </c>
-      <c r="O33" s="11"/>
-      <c r="P33" s="11"/>
-      <c r="Q33" s="11"/>
-      <c r="R33" s="11"/>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B34" s="34"/>
@@ -1966,21 +2306,6 @@
       <c r="I34" s="7">
         <v>7</v>
       </c>
-      <c r="J34" s="11"/>
-      <c r="K34" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="L34" s="28"/>
-      <c r="M34" s="6">
-        <v>96.06</v>
-      </c>
-      <c r="N34" s="20">
-        <v>7</v>
-      </c>
-      <c r="O34" s="11"/>
-      <c r="P34" s="11"/>
-      <c r="Q34" s="11"/>
-      <c r="R34" s="11"/>
     </row>
     <row r="35" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="34" t="s">
@@ -1999,21 +2324,6 @@
       <c r="I35" s="7">
         <v>9</v>
       </c>
-      <c r="J35" s="11"/>
-      <c r="K35" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="L35" s="28"/>
-      <c r="M35" s="6">
-        <v>5.9</v>
-      </c>
-      <c r="N35" s="20">
-        <v>9</v>
-      </c>
-      <c r="O35" s="11"/>
-      <c r="P35" s="11"/>
-      <c r="Q35" s="11"/>
-      <c r="R35" s="11"/>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B36" s="34"/>
@@ -2030,21 +2340,6 @@
       <c r="I36" s="7">
         <v>11</v>
       </c>
-      <c r="J36" s="11"/>
-      <c r="K36" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="L36" s="28"/>
-      <c r="M36" s="6">
-        <v>7.17</v>
-      </c>
-      <c r="N36" s="20">
-        <v>11</v>
-      </c>
-      <c r="O36" s="11"/>
-      <c r="P36" s="11"/>
-      <c r="Q36" s="11"/>
-      <c r="R36" s="11"/>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B37" s="34"/>
@@ -2062,22 +2357,6 @@
       <c r="I37" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="J37" s="11"/>
-      <c r="K37" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="L37" s="27"/>
-      <c r="M37" s="6">
-        <f>SUM(M31:M36, M21)</f>
-        <v>221.84</v>
-      </c>
-      <c r="N37" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="O37" s="11"/>
-      <c r="P37" s="11"/>
-      <c r="Q37" s="11"/>
-      <c r="R37" s="11"/>
     </row>
     <row r="38" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B38" s="34"/>
@@ -2088,34 +2367,15 @@
       <c r="G38" s="4"/>
       <c r="H38" s="3"/>
       <c r="I38" s="1"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="11"/>
-      <c r="L38" s="11"/>
-      <c r="M38" s="11"/>
-      <c r="N38" s="11"/>
-      <c r="O38" s="11"/>
-      <c r="P38" s="11"/>
-      <c r="Q38" s="11"/>
-      <c r="R38" s="11"/>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B39" s="34"/>
       <c r="C39" s="34"/>
       <c r="D39" s="34"/>
       <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
       <c r="G39" s="4"/>
       <c r="H39" s="3"/>
       <c r="I39" s="1"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="11"/>
-      <c r="L39" s="11"/>
-      <c r="M39" s="11"/>
-      <c r="N39" s="11"/>
-      <c r="O39" s="11"/>
-      <c r="P39" s="11"/>
-      <c r="Q39" s="11"/>
-      <c r="R39" s="11"/>
     </row>
     <row r="40" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B40" s="11"/>
@@ -2126,17 +2386,6 @@
       <c r="G40" s="4"/>
       <c r="H40" s="3"/>
       <c r="I40" s="1"/>
-      <c r="J40" s="11"/>
-      <c r="K40" s="11"/>
-      <c r="L40" s="11"/>
-      <c r="M40" s="11"/>
-      <c r="N40" s="11"/>
-      <c r="O40" s="11"/>
-      <c r="P40" s="11"/>
-      <c r="Q40" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="R40" s="11"/>
     </row>
     <row r="41" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B41" s="11"/>
@@ -2391,16 +2640,7 @@
       <c r="D54" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="99">
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="K29:N29"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="K33:L33"/>
+  <mergeCells count="90">
     <mergeCell ref="K21:L21"/>
     <mergeCell ref="O21:T21"/>
     <mergeCell ref="M21:N21"/>
@@ -2512,12 +2752,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A90F1322-9972-45F3-B938-1FA4BAC86127}">
   <dimension ref="A3:T24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3045,7 +3285,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C20" s="10">
         <f>29.5*2</f>

</xml_diff>

<commit_message>
Pushing all schematics to repo
</commit_message>
<xml_diff>
--- a/docs/components.xlsx
+++ b/docs/components.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NAM4SF\Documents\github\adaptive-cruise-control\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897EF3CE-1C17-4186-8E46-216E5CC816C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E9CC6A-B712-4BF3-8AF4-75741722A310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{93B556B3-0F1F-4620-A79F-3801F45D6D88}"/>
+    <workbookView xWindow="-5700" yWindow="-21720" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{93B556B3-0F1F-4620-A79F-3801F45D6D88}"/>
   </bookViews>
   <sheets>
     <sheet name="LinkList" sheetId="3" r:id="rId1"/>
@@ -540,89 +540,89 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -969,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD6834A-62F7-4E19-8029-A60D704C753F}">
   <dimension ref="B2:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11:Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -979,93 +979,93 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="38"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="47" t="s">
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29" t="s">
+      <c r="H3" s="31"/>
+      <c r="I3" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="26" t="s">
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="S3" s="26"/>
+      <c r="S3" s="32"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="48"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="34"/>
       <c r="G4" s="22" t="s">
         <v>11</v>
       </c>
       <c r="H4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="32"/>
+      <c r="S4" s="32"/>
     </row>
     <row r="5" spans="2:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9">
         <v>1</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="49">
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="25">
         <v>1</v>
       </c>
       <c r="G5" s="6">
@@ -1075,63 +1075,63 @@
         <f xml:space="preserve"> G5*1.95</f>
         <v>92.020499999999998</v>
       </c>
-      <c r="I5" s="32" t="s">
+      <c r="I5" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="31"/>
-      <c r="R5" s="23" t="s">
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="S5" s="23"/>
+      <c r="S5" s="29"/>
     </row>
     <row r="6" spans="2:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="9">
         <v>2</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="50"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="26"/>
       <c r="G6" s="6">
         <v>62.9</v>
       </c>
       <c r="H6" s="20">
-        <f t="shared" ref="H6:H12" si="0" xml:space="preserve"> G6*1.95</f>
+        <f t="shared" ref="H6:H9" si="0" xml:space="preserve"> G6*1.95</f>
         <v>122.655</v>
       </c>
-      <c r="I6" s="32" t="s">
+      <c r="I6" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="31"/>
-      <c r="Q6" s="31"/>
-      <c r="R6" s="23" t="s">
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="28"/>
+      <c r="R6" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="S6" s="23"/>
+      <c r="S6" s="29"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B7" s="9">
         <v>3</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="49">
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="25">
         <v>1</v>
       </c>
       <c r="G7" s="6">
@@ -1141,30 +1141,30 @@
         <f t="shared" si="0"/>
         <v>77.804999999999993</v>
       </c>
-      <c r="I7" s="32" t="s">
+      <c r="I7" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="31"/>
-      <c r="O7" s="31"/>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="31"/>
-      <c r="R7" s="23" t="s">
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
+      <c r="R7" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="S7" s="23"/>
+      <c r="S7" s="29"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B8" s="9">
         <v>4</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="50"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="26"/>
       <c r="G8" s="6">
         <f>61.74 / 2</f>
         <v>30.87</v>
@@ -1172,32 +1172,32 @@
       <c r="H8" s="20">
         <v>61.74</v>
       </c>
-      <c r="I8" s="32" t="s">
+      <c r="I8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="31"/>
-      <c r="R8" s="23" t="s">
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="S8" s="23"/>
+      <c r="S8" s="29"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B9" s="9">
         <v>5</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="49">
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="25">
         <v>2</v>
       </c>
       <c r="G9" s="20">
@@ -1207,30 +1207,30 @@
         <f t="shared" si="0"/>
         <v>27.358499999999999</v>
       </c>
-      <c r="I9" s="32" t="s">
+      <c r="I9" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="31"/>
-      <c r="O9" s="31"/>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="31"/>
-      <c r="R9" s="23" t="s">
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="S9" s="23"/>
+      <c r="S9" s="29"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B10" s="9">
         <v>6</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="50"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="26"/>
       <c r="G10" s="6">
         <f>H10/1.95</f>
         <v>13.569230769230771</v>
@@ -1238,32 +1238,32 @@
       <c r="H10" s="20">
         <v>26.46</v>
       </c>
-      <c r="I10" s="32" t="s">
+      <c r="I10" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="31"/>
-      <c r="O10" s="31"/>
-      <c r="P10" s="31"/>
-      <c r="Q10" s="31"/>
-      <c r="R10" s="23" t="s">
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="S10" s="23"/>
+      <c r="S10" s="29"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B11" s="9">
         <v>7</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="49">
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="25">
         <v>1</v>
       </c>
       <c r="G11" s="6">
@@ -1273,30 +1273,30 @@
       <c r="H11" s="20">
         <v>99.41</v>
       </c>
-      <c r="I11" s="32" t="s">
+      <c r="I11" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="31"/>
-      <c r="P11" s="31"/>
-      <c r="Q11" s="31"/>
-      <c r="R11" s="23" t="s">
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28"/>
+      <c r="Q11" s="28"/>
+      <c r="R11" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="S11" s="23"/>
+      <c r="S11" s="29"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B12" s="9">
         <v>8</v>
       </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="50"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="26"/>
       <c r="G12" s="6">
         <f>H12/1.95</f>
         <v>49.261538461538464</v>
@@ -1304,24 +1304,39 @@
       <c r="H12" s="20">
         <v>96.06</v>
       </c>
-      <c r="I12" s="33" t="s">
+      <c r="I12" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="J12" s="33"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="33"/>
-      <c r="O12" s="33"/>
-      <c r="P12" s="33"/>
-      <c r="Q12" s="33"/>
-      <c r="R12" s="23" t="s">
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="30"/>
+      <c r="R12" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="S12" s="23"/>
+      <c r="S12" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="R3:S4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="C5:E6"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:E4"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:Q4"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="I8:Q8"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="I5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="I6:Q6"/>
+    <mergeCell ref="R6:S6"/>
     <mergeCell ref="B2:S2"/>
     <mergeCell ref="C11:E12"/>
     <mergeCell ref="F11:F12"/>
@@ -1338,21 +1353,6 @@
     <mergeCell ref="C7:E8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="I7:Q7"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="I8:Q8"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="I5:Q5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="I6:Q6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="C5:E6"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:E4"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:Q4"/>
-    <mergeCell ref="R3:S4"/>
-    <mergeCell ref="F3:F4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I7" r:id="rId1" xr:uid="{4835562A-740E-44BF-972E-7EE1336F2F12}"/>
@@ -1373,8 +1373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B714DB9D-3D94-4649-9B27-6954336A2F86}">
   <dimension ref="A3:T54"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21:T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1389,44 +1389,44 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29" t="s">
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29" t="s">
+      <c r="I3" s="31"/>
+      <c r="J3" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="26" t="s">
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="T3" s="26"/>
+      <c r="T3" s="32"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="29"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
       <c r="E4" s="14" t="s">
         <v>1</v>
       </c>
@@ -1442,34 +1442,34 @@
       <c r="I4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="26"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="32"/>
+      <c r="T4" s="32"/>
     </row>
     <row r="5" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>1</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="28">
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="36">
         <v>5</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="36">
         <v>1800</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G5" s="36">
         <f xml:space="preserve"> E5*F5/1000</f>
         <v>9</v>
       </c>
@@ -1480,34 +1480,34 @@
         <f xml:space="preserve"> H5*1.95</f>
         <v>134.54999999999998</v>
       </c>
-      <c r="J5" s="32" t="s">
+      <c r="J5" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="31"/>
-      <c r="R5" s="31"/>
-      <c r="S5" s="25" t="s">
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="28"/>
+      <c r="S5" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="T5" s="25"/>
+      <c r="T5" s="41"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>2</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
       <c r="H6" s="6">
         <v>46</v>
       </c>
@@ -1515,38 +1515,38 @@
         <f t="shared" ref="I6:I16" si="0" xml:space="preserve"> H6*1.95</f>
         <v>89.7</v>
       </c>
-      <c r="J6" s="32" t="s">
+      <c r="J6" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="31"/>
-      <c r="Q6" s="31"/>
-      <c r="R6" s="31"/>
-      <c r="S6" s="25" t="s">
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="28"/>
+      <c r="R6" s="28"/>
+      <c r="S6" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="T6" s="25"/>
+      <c r="T6" s="41"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="28">
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="36">
         <v>12</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="36">
         <v>0</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G7" s="36">
         <f t="shared" ref="G7" si="1" xml:space="preserve"> E7*F7/1000</f>
         <v>0</v>
       </c>
@@ -1557,32 +1557,32 @@
         <f t="shared" si="0"/>
         <v>62.750999999999998</v>
       </c>
-      <c r="J7" s="32" t="s">
+      <c r="J7" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="31"/>
-      <c r="O7" s="31"/>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="31"/>
-      <c r="R7" s="31"/>
-      <c r="S7" s="25" t="s">
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
+      <c r="R7" s="28"/>
+      <c r="S7" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="T7" s="25"/>
+      <c r="T7" s="41"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>4</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
       <c r="H8" s="6">
         <f>61.74 / 2</f>
         <v>30.87</v>
@@ -1590,38 +1590,38 @@
       <c r="I8" s="15">
         <v>61.74</v>
       </c>
-      <c r="J8" s="32" t="s">
+      <c r="J8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="31"/>
-      <c r="R8" s="31"/>
-      <c r="S8" s="23" t="s">
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="28"/>
+      <c r="S8" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="T8" s="23"/>
+      <c r="T8" s="29"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>5</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="28">
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="36">
         <v>3.3</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="36">
         <v>300</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="36">
         <f t="shared" ref="G9:G13" si="2" xml:space="preserve"> E9*F9/1000</f>
         <v>0.99</v>
       </c>
@@ -1632,32 +1632,32 @@
         <f t="shared" si="0"/>
         <v>27.358499999999999</v>
       </c>
-      <c r="J9" s="32" t="s">
+      <c r="J9" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="31"/>
-      <c r="O9" s="31"/>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="31"/>
-      <c r="R9" s="31"/>
-      <c r="S9" s="23" t="s">
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="28"/>
+      <c r="S9" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="T9" s="23"/>
+      <c r="T9" s="29"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>6</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
       <c r="H10" s="6">
         <f>I10/1.95</f>
         <v>13.569230769230771</v>
@@ -1665,38 +1665,38 @@
       <c r="I10" s="15">
         <v>26.46</v>
       </c>
-      <c r="J10" s="32" t="s">
+      <c r="J10" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="31"/>
-      <c r="O10" s="31"/>
-      <c r="P10" s="31"/>
-      <c r="Q10" s="31"/>
-      <c r="R10" s="31"/>
-      <c r="S10" s="23" t="s">
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="28"/>
+      <c r="S10" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="T10" s="23"/>
+      <c r="T10" s="29"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>7</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="28">
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="36">
         <v>5.0999999999999996</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="36">
         <v>850</v>
       </c>
-      <c r="G11" s="28">
+      <c r="G11" s="36">
         <f t="shared" si="2"/>
         <v>4.335</v>
       </c>
@@ -1707,32 +1707,32 @@
       <c r="I11" s="15">
         <v>146.58000000000001</v>
       </c>
-      <c r="J11" s="32" t="s">
+      <c r="J11" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="31"/>
-      <c r="P11" s="31"/>
-      <c r="Q11" s="31"/>
-      <c r="R11" s="31"/>
-      <c r="S11" s="23" t="s">
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28"/>
+      <c r="Q11" s="28"/>
+      <c r="R11" s="28"/>
+      <c r="S11" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="T11" s="23"/>
+      <c r="T11" s="29"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>8</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
       <c r="H12" s="6">
         <f>I12/1.95</f>
         <v>49.261538461538464</v>
@@ -1740,38 +1740,38 @@
       <c r="I12" s="15">
         <v>96.06</v>
       </c>
-      <c r="J12" s="33" t="s">
+      <c r="J12" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="33"/>
-      <c r="O12" s="33"/>
-      <c r="P12" s="33"/>
-      <c r="Q12" s="33"/>
-      <c r="R12" s="33"/>
-      <c r="S12" s="25" t="s">
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="30"/>
+      <c r="R12" s="30"/>
+      <c r="S12" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="T12" s="25"/>
+      <c r="T12" s="41"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>9</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="28">
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="36">
         <v>0</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F13" s="36">
         <v>0</v>
       </c>
-      <c r="G13" s="28">
+      <c r="G13" s="36">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1782,32 +1782,32 @@
       <c r="I13" s="15">
         <v>5.9</v>
       </c>
-      <c r="J13" s="32" t="s">
+      <c r="J13" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="31"/>
-      <c r="P13" s="31"/>
-      <c r="Q13" s="31"/>
-      <c r="R13" s="31"/>
-      <c r="S13" s="23" t="s">
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="28"/>
+      <c r="R13" s="28"/>
+      <c r="S13" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="T13" s="23"/>
+      <c r="T13" s="29"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>10</v>
       </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
       <c r="H14" s="6">
         <f>I14/1.95</f>
         <v>1.4871794871794872</v>
@@ -1815,38 +1815,38 @@
       <c r="I14" s="15">
         <v>2.9</v>
       </c>
-      <c r="J14" s="32" t="s">
+      <c r="J14" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="K14" s="31"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="31"/>
-      <c r="O14" s="31"/>
-      <c r="P14" s="31"/>
-      <c r="Q14" s="31"/>
-      <c r="R14" s="31"/>
-      <c r="S14" s="23" t="s">
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="28"/>
+      <c r="R14" s="28"/>
+      <c r="S14" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="T14" s="23"/>
+      <c r="T14" s="29"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>11</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="28" t="s">
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="28" t="s">
+      <c r="F15" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="28" t="s">
+      <c r="G15" s="36" t="s">
         <v>24</v>
       </c>
       <c r="H15" s="6">
@@ -1856,32 +1856,32 @@
         <f t="shared" si="0"/>
         <v>7.1760000000000002</v>
       </c>
-      <c r="J15" s="32" t="s">
+      <c r="J15" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="K15" s="31"/>
-      <c r="L15" s="31"/>
-      <c r="M15" s="31"/>
-      <c r="N15" s="31"/>
-      <c r="O15" s="31"/>
-      <c r="P15" s="31"/>
-      <c r="Q15" s="31"/>
-      <c r="R15" s="31"/>
-      <c r="S15" s="23" t="s">
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="28"/>
+      <c r="R15" s="28"/>
+      <c r="S15" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="T15" s="23"/>
+      <c r="T15" s="29"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>12</v>
       </c>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
       <c r="H16" s="6">
         <v>7.73</v>
       </c>
@@ -1889,29 +1889,29 @@
         <f t="shared" si="0"/>
         <v>15.073500000000001</v>
       </c>
-      <c r="J16" s="32" t="s">
+      <c r="J16" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="K16" s="31"/>
-      <c r="L16" s="31"/>
-      <c r="M16" s="31"/>
-      <c r="N16" s="31"/>
-      <c r="O16" s="31"/>
-      <c r="P16" s="31"/>
-      <c r="Q16" s="31"/>
-      <c r="R16" s="31"/>
-      <c r="S16" s="23" t="s">
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="28"/>
+      <c r="Q16" s="28"/>
+      <c r="R16" s="28"/>
+      <c r="S16" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="T16" s="23"/>
+      <c r="T16" s="29"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
       <c r="E17" s="13" t="s">
         <v>24</v>
       </c>
@@ -1923,30 +1923,30 @@
         <f>SUM(G5:G14)</f>
         <v>14.324999999999999</v>
       </c>
-      <c r="H17" s="36" t="s">
+      <c r="H17" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="I17" s="36"/>
-      <c r="J17" s="31" t="s">
+      <c r="I17" s="39"/>
+      <c r="J17" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="K17" s="31"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="31"/>
-      <c r="N17" s="31"/>
-      <c r="O17" s="31"/>
-      <c r="P17" s="31"/>
-      <c r="Q17" s="31"/>
-      <c r="R17" s="31"/>
-      <c r="S17" s="24" t="s">
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="28"/>
+      <c r="Q17" s="28"/>
+      <c r="R17" s="28"/>
+      <c r="S17" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="T17" s="24"/>
+      <c r="T17" s="42"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -1963,43 +1963,43 @@
       <c r="R18" s="11"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
       <c r="E19" s="4"/>
-      <c r="F19" s="27" t="s">
+      <c r="F19" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
       <c r="J19" s="11"/>
-      <c r="K19" s="29" t="s">
+      <c r="K19" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="L19" s="29"/>
-      <c r="M19" s="29"/>
-      <c r="N19" s="29"/>
-      <c r="O19" s="29"/>
-      <c r="P19" s="29"/>
-      <c r="Q19" s="29"/>
-      <c r="R19" s="29"/>
-      <c r="S19" s="29"/>
-      <c r="T19" s="29"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="31"/>
+      <c r="N19" s="31"/>
+      <c r="O19" s="31"/>
+      <c r="P19" s="31"/>
+      <c r="Q19" s="31"/>
+      <c r="R19" s="31"/>
+      <c r="S19" s="31"/>
+      <c r="T19" s="31"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B20" s="37" t="s">
+      <c r="B20" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
       <c r="E20" s="4"/>
-      <c r="F20" s="27" t="s">
+      <c r="F20" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="G20" s="27"/>
+      <c r="G20" s="35"/>
       <c r="H20" s="8" t="s">
         <v>33</v>
       </c>
@@ -2007,34 +2007,34 @@
         <v>34</v>
       </c>
       <c r="J20" s="11"/>
-      <c r="K20" s="29" t="s">
+      <c r="K20" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="L20" s="29"/>
-      <c r="M20" s="29" t="s">
+      <c r="L20" s="31"/>
+      <c r="M20" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="N20" s="29"/>
-      <c r="O20" s="29" t="s">
+      <c r="N20" s="31"/>
+      <c r="O20" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="P20" s="29"/>
-      <c r="Q20" s="29"/>
-      <c r="R20" s="29"/>
-      <c r="S20" s="29"/>
-      <c r="T20" s="29"/>
+      <c r="P20" s="31"/>
+      <c r="Q20" s="31"/>
+      <c r="R20" s="31"/>
+      <c r="S20" s="31"/>
+      <c r="T20" s="31"/>
     </row>
     <row r="21" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="28" t="s">
+      <c r="F21" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="G21" s="28"/>
+      <c r="G21" s="36"/>
       <c r="H21" s="6">
         <v>134.55000000000001</v>
       </c>
@@ -2042,32 +2042,32 @@
         <v>1</v>
       </c>
       <c r="J21" s="11"/>
-      <c r="K21" s="31" t="s">
+      <c r="K21" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="L21" s="31"/>
-      <c r="M21" s="31">
+      <c r="L21" s="28"/>
+      <c r="M21" s="28">
         <v>22.91</v>
       </c>
-      <c r="N21" s="31"/>
-      <c r="O21" s="32" t="s">
+      <c r="N21" s="28"/>
+      <c r="O21" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="P21" s="31"/>
-      <c r="Q21" s="31"/>
-      <c r="R21" s="31"/>
-      <c r="S21" s="31"/>
-      <c r="T21" s="31"/>
+      <c r="P21" s="28"/>
+      <c r="Q21" s="28"/>
+      <c r="R21" s="28"/>
+      <c r="S21" s="28"/>
+      <c r="T21" s="28"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
       <c r="E22" s="4"/>
-      <c r="F22" s="28" t="s">
+      <c r="F22" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="G22" s="28"/>
+      <c r="G22" s="36"/>
       <c r="H22" s="6">
         <v>61.74</v>
       </c>
@@ -2085,14 +2085,14 @@
       <c r="R22" s="11"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="28" t="s">
+      <c r="F23" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="G23" s="28"/>
+      <c r="G23" s="36"/>
       <c r="H23" s="6">
         <f>14.03 * 2</f>
         <v>28.06</v>
@@ -2111,16 +2111,16 @@
       <c r="R23" s="11"/>
     </row>
     <row r="24" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="34" t="s">
+      <c r="B24" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
       <c r="E24" s="4"/>
-      <c r="F24" s="28" t="s">
+      <c r="F24" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="G24" s="28"/>
+      <c r="G24" s="36"/>
       <c r="H24" s="6">
         <v>96.06</v>
       </c>
@@ -2138,14 +2138,14 @@
       <c r="R24" s="11"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
       <c r="E25" s="4"/>
-      <c r="F25" s="28" t="s">
+      <c r="F25" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="G25" s="28"/>
+      <c r="G25" s="36"/>
       <c r="H25" s="6">
         <v>5.9</v>
       </c>
@@ -2163,14 +2163,14 @@
       <c r="R25" s="11"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B26" s="34"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
       <c r="E26" s="4"/>
-      <c r="F26" s="28" t="s">
+      <c r="F26" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="G26" s="28"/>
+      <c r="G26" s="36"/>
       <c r="H26" s="6">
         <v>7.17</v>
       </c>
@@ -2188,14 +2188,14 @@
       <c r="R26" s="11"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
       <c r="E27" s="4"/>
-      <c r="F27" s="27" t="s">
+      <c r="F27" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="G27" s="27"/>
+      <c r="G27" s="35"/>
       <c r="H27" s="6">
         <f>SUM(H21:H26)</f>
         <v>333.48</v>
@@ -2205,9 +2205,9 @@
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
@@ -2215,26 +2215,26 @@
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
       <c r="E29" s="4"/>
-      <c r="F29" s="27" t="s">
+      <c r="F29" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="35"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
       <c r="E30" s="4"/>
-      <c r="F30" s="27" t="s">
+      <c r="F30" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="G30" s="27"/>
+      <c r="G30" s="35"/>
       <c r="H30" s="8" t="s">
         <v>33</v>
       </c>
@@ -2243,14 +2243,14 @@
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
       <c r="E31" s="4"/>
-      <c r="F31" s="28" t="s">
+      <c r="F31" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="G31" s="28"/>
+      <c r="G31" s="36"/>
       <c r="H31" s="6">
         <v>89.7</v>
       </c>
@@ -2259,14 +2259,14 @@
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
       <c r="E32" s="4"/>
-      <c r="F32" s="28" t="s">
+      <c r="F32" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="G32" s="28"/>
+      <c r="G32" s="36"/>
       <c r="H32" s="6">
         <v>61.74</v>
       </c>
@@ -2275,14 +2275,14 @@
       </c>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
       <c r="E33" s="4"/>
-      <c r="F33" s="28" t="s">
+      <c r="F33" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="G33" s="28"/>
+      <c r="G33" s="36"/>
       <c r="H33" s="6">
         <f xml:space="preserve"> 14.03 * 2</f>
         <v>28.06</v>
@@ -2292,14 +2292,14 @@
       </c>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B34" s="34"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="37"/>
       <c r="E34" s="4"/>
-      <c r="F34" s="28" t="s">
+      <c r="F34" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="28"/>
+      <c r="G34" s="36"/>
       <c r="H34" s="6">
         <v>98.65</v>
       </c>
@@ -2308,16 +2308,16 @@
       </c>
     </row>
     <row r="35" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="34" t="s">
+      <c r="B35" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="34"/>
-      <c r="D35" s="34"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
       <c r="E35" s="4"/>
-      <c r="F35" s="28" t="s">
+      <c r="F35" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="G35" s="28"/>
+      <c r="G35" s="36"/>
       <c r="H35" s="6">
         <v>5.9</v>
       </c>
@@ -2326,14 +2326,14 @@
       </c>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B36" s="34"/>
-      <c r="C36" s="34"/>
-      <c r="D36" s="34"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="37"/>
+      <c r="D36" s="37"/>
       <c r="E36" s="4"/>
-      <c r="F36" s="28" t="s">
+      <c r="F36" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="G36" s="28"/>
+      <c r="G36" s="36"/>
       <c r="H36" s="6">
         <v>7.17</v>
       </c>
@@ -2342,14 +2342,14 @@
       </c>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B37" s="34"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="34"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37"/>
       <c r="E37" s="4"/>
-      <c r="F37" s="27" t="s">
+      <c r="F37" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="G37" s="27"/>
+      <c r="G37" s="35"/>
       <c r="H37" s="6">
         <f>SUM(H31:H36, M21)</f>
         <v>314.13</v>
@@ -2359,9 +2359,9 @@
       </c>
     </row>
     <row r="38" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B38" s="34"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="34"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="37"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
@@ -2369,9 +2369,9 @@
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B39" s="34"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="37"/>
       <c r="E39" s="4"/>
       <c r="G39" s="4"/>
       <c r="H39" s="3"/>
@@ -2641,30 +2641,56 @@
     </row>
   </sheetData>
   <mergeCells count="90">
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="O21:T21"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="K19:T19"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="O20:T20"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="B7:D8"/>
-    <mergeCell ref="B11:D12"/>
-    <mergeCell ref="B15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="J3:R4"/>
-    <mergeCell ref="J5:R5"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="J6:R6"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="S16:T16"/>
+    <mergeCell ref="S17:T17"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="S11:T11"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="S3:T4"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B3:D4"/>
+    <mergeCell ref="B9:D10"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="J7:R7"/>
+    <mergeCell ref="J8:R8"/>
+    <mergeCell ref="J9:R9"/>
+    <mergeCell ref="J10:R10"/>
+    <mergeCell ref="J11:R11"/>
     <mergeCell ref="J12:R12"/>
     <mergeCell ref="B35:D39"/>
     <mergeCell ref="J17:R17"/>
@@ -2681,56 +2707,30 @@
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B21:D23"/>
     <mergeCell ref="B24:D34"/>
-    <mergeCell ref="J7:R7"/>
-    <mergeCell ref="J8:R8"/>
-    <mergeCell ref="J9:R9"/>
-    <mergeCell ref="J10:R10"/>
-    <mergeCell ref="J11:R11"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B3:D4"/>
-    <mergeCell ref="B9:D10"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="S3:T4"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="S14:T14"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="S16:T16"/>
-    <mergeCell ref="S17:T17"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="S11:T11"/>
-    <mergeCell ref="S12:T12"/>
-    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="J3:R4"/>
+    <mergeCell ref="J5:R5"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="J6:R6"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="B7:D8"/>
+    <mergeCell ref="B11:D12"/>
+    <mergeCell ref="B15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="O21:T21"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="K19:T19"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="O20:T20"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J5" r:id="rId1" xr:uid="{E6C453EF-44A0-4AA5-8DDB-03942D4436C1}"/>
@@ -2770,44 +2770,44 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29" t="s">
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29" t="s">
+      <c r="I3" s="31"/>
+      <c r="J3" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="26" t="s">
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="T3" s="26"/>
+      <c r="T3" s="32"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="29"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
       <c r="E4" s="14" t="s">
         <v>1</v>
       </c>
@@ -2823,34 +2823,34 @@
       <c r="I4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="26"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="32"/>
+      <c r="T4" s="32"/>
     </row>
     <row r="5" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="39">
+      <c r="A5" s="49">
         <v>1</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="28">
+      <c r="C5" s="44"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="36">
         <v>5</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="36">
         <v>3000</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G5" s="36">
         <f xml:space="preserve"> E5*F5/1000</f>
         <v>15</v>
       </c>
@@ -2861,30 +2861,30 @@
         <f xml:space="preserve"> H5*1.95</f>
         <v>134.47199999999998</v>
       </c>
-      <c r="J5" s="32" t="s">
+      <c r="J5" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="31"/>
-      <c r="R5" s="31"/>
-      <c r="S5" s="25" t="s">
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="28"/>
+      <c r="S5" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="T5" s="25"/>
+      <c r="T5" s="41"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" s="40"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
+      <c r="A6" s="50"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
       <c r="H6" s="6">
         <v>56</v>
       </c>
@@ -2892,31 +2892,31 @@
         <f t="shared" ref="I6:I14" si="0" xml:space="preserve"> H6*1.95</f>
         <v>109.2</v>
       </c>
-      <c r="J6" s="32" t="s">
+      <c r="J6" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="31"/>
-      <c r="Q6" s="31"/>
-      <c r="R6" s="31"/>
-      <c r="S6" s="25" t="s">
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="28"/>
+      <c r="R6" s="28"/>
+      <c r="S6" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="T6" s="25"/>
+      <c r="T6" s="41"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>2</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
       <c r="E7" s="12">
         <v>5</v>
       </c>
@@ -2934,31 +2934,31 @@
         <f t="shared" si="0"/>
         <v>45.103499999999997</v>
       </c>
-      <c r="J7" s="32" t="s">
+      <c r="J7" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="31"/>
-      <c r="O7" s="31"/>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="31"/>
-      <c r="R7" s="31"/>
-      <c r="S7" s="23" t="s">
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
+      <c r="R7" s="28"/>
+      <c r="S7" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="T7" s="23"/>
+      <c r="T7" s="29"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>3</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
       <c r="E8" s="12">
         <v>5</v>
       </c>
@@ -2976,38 +2976,38 @@
         <f t="shared" si="0"/>
         <v>29.503500000000003</v>
       </c>
-      <c r="J8" s="32" t="s">
+      <c r="J8" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="31"/>
-      <c r="R8" s="31"/>
-      <c r="S8" s="23" t="s">
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="28"/>
+      <c r="S8" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="T8" s="23"/>
+      <c r="T8" s="29"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>4</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="28">
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="36">
         <v>5.0999999999999996</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="36">
         <v>850</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="36">
         <f t="shared" ref="G9:G11" si="2" xml:space="preserve"> E9*F9/1000</f>
         <v>4.335</v>
       </c>
@@ -3018,32 +3018,32 @@
       <c r="I9" s="15">
         <v>146.58000000000001</v>
       </c>
-      <c r="J9" s="32" t="s">
+      <c r="J9" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="31"/>
-      <c r="O9" s="31"/>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="31"/>
-      <c r="R9" s="31"/>
-      <c r="S9" s="23" t="s">
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="28"/>
+      <c r="S9" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="T9" s="23"/>
+      <c r="T9" s="29"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>5</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
       <c r="H10" s="6">
         <f>I10/1.95</f>
         <v>50.589743589743591</v>
@@ -3051,38 +3051,38 @@
       <c r="I10" s="15">
         <v>98.65</v>
       </c>
-      <c r="J10" s="33" t="s">
+      <c r="J10" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="31"/>
-      <c r="O10" s="31"/>
-      <c r="P10" s="31"/>
-      <c r="Q10" s="31"/>
-      <c r="R10" s="31"/>
-      <c r="S10" s="23" t="s">
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="28"/>
+      <c r="S10" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="T10" s="23"/>
+      <c r="T10" s="29"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>6</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="28">
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="36">
         <v>0</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="36">
         <v>0</v>
       </c>
-      <c r="G11" s="28">
+      <c r="G11" s="36">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3093,32 +3093,32 @@
       <c r="I11" s="15">
         <v>5.9</v>
       </c>
-      <c r="J11" s="32" t="s">
+      <c r="J11" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="31"/>
-      <c r="P11" s="31"/>
-      <c r="Q11" s="31"/>
-      <c r="R11" s="31"/>
-      <c r="S11" s="23" t="s">
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28"/>
+      <c r="Q11" s="28"/>
+      <c r="R11" s="28"/>
+      <c r="S11" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="T11" s="23"/>
+      <c r="T11" s="29"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>7</v>
       </c>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
       <c r="H12" s="6">
         <f>I12/1.95</f>
         <v>1.4871794871794872</v>
@@ -3126,38 +3126,38 @@
       <c r="I12" s="15">
         <v>2.9</v>
       </c>
-      <c r="J12" s="32" t="s">
+      <c r="J12" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
-      <c r="O12" s="31"/>
-      <c r="P12" s="31"/>
-      <c r="Q12" s="31"/>
-      <c r="R12" s="31"/>
-      <c r="S12" s="23" t="s">
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
+      <c r="Q12" s="28"/>
+      <c r="R12" s="28"/>
+      <c r="S12" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="T12" s="23"/>
+      <c r="T12" s="29"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>8</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="28" t="s">
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="F13" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="28" t="s">
+      <c r="G13" s="36" t="s">
         <v>24</v>
       </c>
       <c r="H13" s="6">
@@ -3167,32 +3167,32 @@
         <f t="shared" si="0"/>
         <v>36.270000000000003</v>
       </c>
-      <c r="J13" s="32" t="s">
+      <c r="J13" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="31"/>
-      <c r="P13" s="31"/>
-      <c r="Q13" s="31"/>
-      <c r="R13" s="31"/>
-      <c r="S13" s="25" t="s">
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="28"/>
+      <c r="R13" s="28"/>
+      <c r="S13" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="T13" s="25"/>
+      <c r="T13" s="41"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>9</v>
       </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
       <c r="H14" s="6">
         <v>7.73</v>
       </c>
@@ -3200,29 +3200,29 @@
         <f t="shared" si="0"/>
         <v>15.073500000000001</v>
       </c>
-      <c r="J14" s="32" t="s">
+      <c r="J14" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="K14" s="31"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="31"/>
-      <c r="O14" s="31"/>
-      <c r="P14" s="31"/>
-      <c r="Q14" s="31"/>
-      <c r="R14" s="31"/>
-      <c r="S14" s="23" t="s">
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="28"/>
+      <c r="R14" s="28"/>
+      <c r="S14" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="T14" s="23"/>
+      <c r="T14" s="29"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="17"/>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
       <c r="E15" s="13" t="s">
         <v>24</v>
       </c>
@@ -3234,32 +3234,32 @@
         <f>SUM(G5:G12)</f>
         <v>22.335000000000001</v>
       </c>
-      <c r="H15" s="36" t="s">
+      <c r="H15" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="36"/>
-      <c r="J15" s="31" t="s">
+      <c r="I15" s="39"/>
+      <c r="J15" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="K15" s="31"/>
-      <c r="L15" s="31"/>
-      <c r="M15" s="31"/>
-      <c r="N15" s="31"/>
-      <c r="O15" s="31"/>
-      <c r="P15" s="31"/>
-      <c r="Q15" s="31"/>
-      <c r="R15" s="31"/>
-      <c r="S15" s="24" t="s">
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="28"/>
+      <c r="R15" s="28"/>
+      <c r="S15" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="T15" s="24"/>
+      <c r="T15" s="42"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="18" t="s">
@@ -3340,33 +3340,13 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="S3:T4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:D4"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:R4"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="J8:R8"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="J5:R5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="J6:R6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="S11:T11"/>
-    <mergeCell ref="J12:R12"/>
-    <mergeCell ref="S12:T12"/>
-    <mergeCell ref="B9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="J9:R9"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="J10:R10"/>
-    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J15:R15"/>
+    <mergeCell ref="J11:R11"/>
+    <mergeCell ref="J7:R7"/>
     <mergeCell ref="S15:T15"/>
     <mergeCell ref="B5:D6"/>
     <mergeCell ref="B7:D7"/>
@@ -3383,13 +3363,33 @@
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="G11:G12"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="J15:R15"/>
-    <mergeCell ref="J11:R11"/>
-    <mergeCell ref="J7:R7"/>
+    <mergeCell ref="S11:T11"/>
+    <mergeCell ref="J12:R12"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="B9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="J9:R9"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="J10:R10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="J8:R8"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="J5:R5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="J6:R6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="S3:T4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:D4"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:R4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J5" r:id="rId1" xr:uid="{BAC2EE8B-B72D-4997-B232-439FFEE0FBFD}"/>

</xml_diff>